<commit_message>
power_circles.xlsx: Implement fixes from all issues
- #5 - switched recency sort order
- #6 - tweak recency conditional formatting rules
- #7 - rebuild recency formula to (hopefully) be backward-compatible to
  Excel 2003, and add guardrails for blank date (to show -100% recency)
</commit_message>
<xml_diff>
--- a/power_circles.xlsx
+++ b/power_circles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raman/Dropbox/b/r/contector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D6301-FD55-604D-909B-90FF08978D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D98431-F547-EF4D-99FF-A6C926345D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="840" windowWidth="20560" windowHeight="17460" xr2:uid="{3BBFB18D-8494-554C-A2CC-0F43D995C09A}"/>
+    <workbookView xWindow="3680" yWindow="540" windowWidth="20560" windowHeight="17460" xr2:uid="{3BBFB18D-8494-554C-A2CC-0F43D995C09A}"/>
   </bookViews>
   <sheets>
     <sheet name="power_circles" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -592,406 +586,14 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top style="thin">
-          <color theme="2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="2"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1037,36 +639,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1074,6 +646,27 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1417,7 +1010,7 @@
   <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,21 +1047,21 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E2" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D2) / VLOOKUP(C2, tiers, 2, FALSE), "")</f>
-        <v>0.85714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C2, tiers, 2, FALSE)), "", IF(ISBLANK(D2), -1, 1 - (TODAY() - D2) / VLOOKUP(C2, tiers, 2, FALSE)))</f>
+        <v>-0.14285714285714279</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5"/>
@@ -1478,21 +1071,21 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" s="1">
-        <f ca="1">TODAY() - 2</f>
-        <v>44098</v>
+        <f ca="1">TODAY() - 6</f>
+        <v>44167</v>
       </c>
       <c r="E3" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D3) / VLOOKUP(C3, tiers, 2, FALSE), "")</f>
-        <v>0.7142857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C3, tiers, 2, FALSE)), "", IF(ISBLANK(D3), -1, 1 - (TODAY() - D3) / VLOOKUP(C3, tiers, 2, FALSE)))</f>
+        <v>0.1428571428571429</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
@@ -1502,21 +1095,21 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="1">
         <f ca="1">TODAY() - 2</f>
-        <v>44098</v>
+        <v>44171</v>
       </c>
       <c r="E4" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D4) / VLOOKUP(C4, tiers, 2, FALSE), "")</f>
+        <f ca="1">IF(ISNA(VLOOKUP(C4, tiers, 2, FALSE)), "", IF(ISBLANK(D4), -1, 1 - (TODAY() - D4) / VLOOKUP(C4, tiers, 2, FALSE)))</f>
         <v>0.7142857142857143</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="5"/>
@@ -1526,18 +1119,18 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <f ca="1">TODAY() - 6</f>
-        <v>44094</v>
+        <f ca="1">TODAY() - 2</f>
+        <v>44171</v>
       </c>
       <c r="E5" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D5) / VLOOKUP(C5, tiers, 2, FALSE), "")</f>
-        <v>0.1428571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C5, tiers, 2, FALSE)), "", IF(ISBLANK(D5), -1, 1 - (TODAY() - D5) / VLOOKUP(C5, tiers, 2, FALSE)))</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -1550,21 +1143,21 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E6" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D6) / VLOOKUP(C6, tiers, 2, FALSE), "")</f>
-        <v>-0.14285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C6, tiers, 2, FALSE)), "", IF(ISBLANK(D6), -1, 1 - (TODAY() - D6) / VLOOKUP(C6, tiers, 2, FALSE)))</f>
+        <v>0.85714285714285721</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
@@ -1574,21 +1167,21 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 31</f>
+        <v>44142</v>
       </c>
       <c r="E7" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D7) / VLOOKUP(C7, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C7, tiers, 2, FALSE)), "", IF(ISBLANK(D7), -1, 1 - (TODAY() - D7) / VLOOKUP(C7, tiers, 2, FALSE)))</f>
+        <v>-0.10714285714285721</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
@@ -1598,21 +1191,21 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 27</f>
+        <v>44146</v>
       </c>
       <c r="E8" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D8) / VLOOKUP(C8, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C8, tiers, 2, FALSE)), "", IF(ISBLANK(D8), -1, 1 - (TODAY() - D8) / VLOOKUP(C8, tiers, 2, FALSE)))</f>
+        <v>3.5714285714285698E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
@@ -1622,21 +1215,21 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 25</f>
+        <v>44148</v>
       </c>
       <c r="E9" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D9) / VLOOKUP(C9, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C9, tiers, 2, FALSE)), "", IF(ISBLANK(D9), -1, 1 - (TODAY() - D9) / VLOOKUP(C9, tiers, 2, FALSE)))</f>
+        <v>0.1071428571428571</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
@@ -1646,21 +1239,21 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E10" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D10) / VLOOKUP(C10, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C10, tiers, 2, FALSE)), "", IF(ISBLANK(D10), -1, 1 - (TODAY() - D10) / VLOOKUP(C10, tiers, 2, FALSE)))</f>
+        <v>0.3571428571428571</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
@@ -1670,21 +1263,21 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 14</f>
+        <v>44159</v>
       </c>
       <c r="E11" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D11) / VLOOKUP(C11, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C11, tiers, 2, FALSE)), "", IF(ISBLANK(D11), -1, 1 - (TODAY() - D11) / VLOOKUP(C11, tiers, 2, FALSE)))</f>
+        <v>0.5</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
@@ -1694,21 +1287,21 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 14</f>
+        <v>44159</v>
       </c>
       <c r="E12" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D12) / VLOOKUP(C12, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C12, tiers, 2, FALSE)), "", IF(ISBLANK(D12), -1, 1 - (TODAY() - D12) / VLOOKUP(C12, tiers, 2, FALSE)))</f>
+        <v>0.5</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="5"/>
@@ -1718,18 +1311,18 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 14</f>
+        <v>44159</v>
       </c>
       <c r="E13" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D13) / VLOOKUP(C13, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C13, tiers, 2, FALSE)), "", IF(ISBLANK(D13), -1, 1 - (TODAY() - D13) / VLOOKUP(C13, tiers, 2, FALSE)))</f>
+        <v>0.5</v>
       </c>
       <c r="F13" t="s">
         <v>39</v>
@@ -1742,18 +1335,18 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="1">
-        <f ca="1">TODAY() - 2</f>
-        <v>44098</v>
+        <f ca="1">TODAY() - 13</f>
+        <v>44160</v>
       </c>
       <c r="E14" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D14) / VLOOKUP(C14, tiers, 2, FALSE), "")</f>
-        <v>0.9285714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C14, tiers, 2, FALSE)), "", IF(ISBLANK(D14), -1, 1 - (TODAY() - D14) / VLOOKUP(C14, tiers, 2, FALSE)))</f>
+        <v>0.5357142857142857</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -1766,21 +1359,21 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <f ca="1">TODAY() - 4</f>
-        <v>44096</v>
+        <f ca="1">TODAY() - 10</f>
+        <v>44163</v>
       </c>
       <c r="E15" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D15) / VLOOKUP(C15, tiers, 2, FALSE), "")</f>
-        <v>0.85714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C15, tiers, 2, FALSE)), "", IF(ISBLANK(D15), -1, 1 - (TODAY() - D15) / VLOOKUP(C15, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="5"/>
@@ -1790,21 +1383,21 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" s="1">
-        <f ca="1">TODAY() - 4</f>
-        <v>44096</v>
+        <f ca="1">TODAY() - 10</f>
+        <v>44163</v>
       </c>
       <c r="E16" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D16) / VLOOKUP(C16, tiers, 2, FALSE), "")</f>
-        <v>0.85714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C16, tiers, 2, FALSE)), "", IF(ISBLANK(D16), -1, 1 - (TODAY() - D16) / VLOOKUP(C16, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="5"/>
@@ -1814,21 +1407,21 @@
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <f ca="1">TODAY() - 9</f>
+        <v>44164</v>
       </c>
       <c r="E17" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D17) / VLOOKUP(C17, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C17, tiers, 2, FALSE)), "", IF(ISBLANK(D17), -1, 1 - (TODAY() - D17) / VLOOKUP(C17, tiers, 2, FALSE)))</f>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="5"/>
@@ -1838,21 +1431,21 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E18" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D18) / VLOOKUP(C18, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C18, tiers, 2, FALSE)), "", IF(ISBLANK(D18), -1, 1 - (TODAY() - D18) / VLOOKUP(C18, tiers, 2, FALSE)))</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="5"/>
@@ -1862,21 +1455,21 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" s="1">
         <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <v>44168</v>
       </c>
       <c r="E19" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D19) / VLOOKUP(C19, tiers, 2, FALSE), "")</f>
+        <f ca="1">IF(ISNA(VLOOKUP(C19, tiers, 2, FALSE)), "", IF(ISBLANK(D19), -1, 1 - (TODAY() - D19) / VLOOKUP(C19, tiers, 2, FALSE)))</f>
         <v>0.8214285714285714</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5"/>
@@ -1886,21 +1479,21 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 5</f>
+        <v>44168</v>
       </c>
       <c r="E20" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D20) / VLOOKUP(C20, tiers, 2, FALSE), "")</f>
-        <v>0.7142857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C20, tiers, 2, FALSE)), "", IF(ISBLANK(D20), -1, 1 - (TODAY() - D20) / VLOOKUP(C20, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="5"/>
@@ -1910,21 +1503,21 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <f ca="1">TODAY() - 9</f>
-        <v>44091</v>
+        <f ca="1">TODAY() - 5</f>
+        <v>44168</v>
       </c>
       <c r="E21" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D21) / VLOOKUP(C21, tiers, 2, FALSE), "")</f>
-        <v>0.6785714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C21, tiers, 2, FALSE)), "", IF(ISBLANK(D21), -1, 1 - (TODAY() - D21) / VLOOKUP(C21, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F21" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="5"/>
@@ -1934,21 +1527,21 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <f ca="1">TODAY() - 10</f>
-        <v>44090</v>
+        <f ca="1">TODAY() - 4</f>
+        <v>44169</v>
       </c>
       <c r="E22" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D22) / VLOOKUP(C22, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C22, tiers, 2, FALSE)), "", IF(ISBLANK(D22), -1, 1 - (TODAY() - D22) / VLOOKUP(C22, tiers, 2, FALSE)))</f>
+        <v>0.85714285714285721</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="5"/>
@@ -1958,21 +1551,21 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <f ca="1">TODAY() - 10</f>
-        <v>44090</v>
+        <f ca="1">TODAY() - 4</f>
+        <v>44169</v>
       </c>
       <c r="E23" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D23) / VLOOKUP(C23, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C23, tiers, 2, FALSE)), "", IF(ISBLANK(D23), -1, 1 - (TODAY() - D23) / VLOOKUP(C23, tiers, 2, FALSE)))</f>
+        <v>0.85714285714285721</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="5"/>
@@ -1982,18 +1575,18 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <f ca="1">TODAY() - 13</f>
-        <v>44087</v>
+        <f ca="1">TODAY() - 2</f>
+        <v>44171</v>
       </c>
       <c r="E24" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D24) / VLOOKUP(C24, tiers, 2, FALSE), "")</f>
-        <v>0.5357142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C24, tiers, 2, FALSE)), "", IF(ISBLANK(D24), -1, 1 - (TODAY() - D24) / VLOOKUP(C24, tiers, 2, FALSE)))</f>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
@@ -2006,21 +1599,21 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <f ca="1">TODAY() - 14</f>
-        <v>44086</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E25" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D25) / VLOOKUP(C25, tiers, 2, FALSE), "")</f>
-        <v>0.5</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C25, tiers, 2, FALSE)), "", IF(ISBLANK(D25), -1, 1 - (TODAY() - D25) / VLOOKUP(C25, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="5"/>
@@ -2030,21 +1623,21 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <f ca="1">TODAY() - 14</f>
-        <v>44086</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E26" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D26) / VLOOKUP(C26, tiers, 2, FALSE), "")</f>
-        <v>0.5</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C26, tiers, 2, FALSE)), "", IF(ISBLANK(D26), -1, 1 - (TODAY() - D26) / VLOOKUP(C26, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="5"/>
@@ -2054,21 +1647,21 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <f ca="1">TODAY() - 14</f>
-        <v>44086</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E27" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D27) / VLOOKUP(C27, tiers, 2, FALSE), "")</f>
-        <v>0.5</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C27, tiers, 2, FALSE)), "", IF(ISBLANK(D27), -1, 1 - (TODAY() - D27) / VLOOKUP(C27, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="5"/>
@@ -2078,21 +1671,21 @@
         <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E28" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D28) / VLOOKUP(C28, tiers, 2, FALSE), "")</f>
-        <v>0.3571428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C28, tiers, 2, FALSE)), "", IF(ISBLANK(D28), -1, 1 - (TODAY() - D28) / VLOOKUP(C28, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F28" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="5"/>
@@ -2102,21 +1695,21 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <f ca="1">TODAY() - 25</f>
-        <v>44075</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E29" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D29) / VLOOKUP(C29, tiers, 2, FALSE), "")</f>
-        <v>0.1071428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C29, tiers, 2, FALSE)), "", IF(ISBLANK(D29), -1, 1 - (TODAY() - D29) / VLOOKUP(C29, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="5"/>
@@ -2126,21 +1719,21 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <f ca="1">TODAY() - 27</f>
-        <v>44073</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E30" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D30) / VLOOKUP(C30, tiers, 2, FALSE), "")</f>
-        <v>3.5714285714285698E-2</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C30, tiers, 2, FALSE)), "", IF(ISBLANK(D30), -1, 1 - (TODAY() - D30) / VLOOKUP(C30, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="5"/>
@@ -2150,21 +1743,21 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <f ca="1">TODAY() - 31</f>
-        <v>44069</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E31" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D31) / VLOOKUP(C31, tiers, 2, FALSE), "")</f>
-        <v>-0.10714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C31, tiers, 2, FALSE)), "", IF(ISBLANK(D31), -1, 1 - (TODAY() - D31) / VLOOKUP(C31, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="5"/>
@@ -2174,21 +1767,21 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 108</f>
+        <v>44065</v>
       </c>
       <c r="E32" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D32) / VLOOKUP(C32, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C32, tiers, 2, FALSE)), "", IF(ISBLANK(D32), -1, 1 - (TODAY() - D32) / VLOOKUP(C32, tiers, 2, FALSE)))</f>
+        <v>3.5714285714285698E-2</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="5"/>
@@ -2198,21 +1791,21 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 102</f>
+        <v>44071</v>
       </c>
       <c r="E33" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D33) / VLOOKUP(C33, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C33, tiers, 2, FALSE)), "", IF(ISBLANK(D33), -1, 1 - (TODAY() - D33) / VLOOKUP(C33, tiers, 2, FALSE)))</f>
+        <v>8.9285714285714302E-2</v>
       </c>
       <c r="F33" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="5"/>
@@ -2222,21 +1815,21 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34">
+        <v>149</v>
+      </c>
+      <c r="C34" s="2">
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 97</f>
+        <v>44076</v>
       </c>
       <c r="E34" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D34) / VLOOKUP(C34, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C34, tiers, 2, FALSE)), "", IF(ISBLANK(D34), -1, 1 - (TODAY() - D34) / VLOOKUP(C34, tiers, 2, FALSE)))</f>
+        <v>0.1339285714285714</v>
       </c>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="5"/>
@@ -2246,21 +1839,21 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" s="1">
-        <f ca="1">TODAY() - 0</f>
-        <v>44100</v>
+        <f ca="1">TODAY() - 94</f>
+        <v>44079</v>
       </c>
       <c r="E35" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D35) / VLOOKUP(C35, tiers, 2, FALSE), "")</f>
-        <v>1</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C35, tiers, 2, FALSE)), "", IF(ISBLANK(D35), -1, 1 - (TODAY() - D35) / VLOOKUP(C35, tiers, 2, FALSE)))</f>
+        <v>0.1607142857142857</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="5"/>
@@ -2270,21 +1863,21 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 90</f>
+        <v>44083</v>
       </c>
       <c r="E36" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D36) / VLOOKUP(C36, tiers, 2, FALSE), "")</f>
-        <v>0.9910714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C36, tiers, 2, FALSE)), "", IF(ISBLANK(D36), -1, 1 - (TODAY() - D36) / VLOOKUP(C36, tiers, 2, FALSE)))</f>
+        <v>0.1964285714285714</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="5"/>
@@ -2294,21 +1887,21 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" s="1">
-        <f ca="1">TODAY() - 1</f>
-        <v>44099</v>
+        <f ca="1">TODAY() - 86</f>
+        <v>44087</v>
       </c>
       <c r="E37" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D37) / VLOOKUP(C37, tiers, 2, FALSE), "")</f>
-        <v>0.9910714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C37, tiers, 2, FALSE)), "", IF(ISBLANK(D37), -1, 1 - (TODAY() - D37) / VLOOKUP(C37, tiers, 2, FALSE)))</f>
+        <v>0.2321428571428571</v>
       </c>
       <c r="F37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="5"/>
@@ -2318,21 +1911,21 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="2">
+        <v>145</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" s="1">
-        <f ca="1">TODAY() - 3</f>
-        <v>44097</v>
+        <f ca="1">TODAY() - 82</f>
+        <v>44091</v>
       </c>
       <c r="E38" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D38) / VLOOKUP(C38, tiers, 2, FALSE), "")</f>
-        <v>0.9732142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C38, tiers, 2, FALSE)), "", IF(ISBLANK(D38), -1, 1 - (TODAY() - D38) / VLOOKUP(C38, tiers, 2, FALSE)))</f>
+        <v>0.2678571428571429</v>
       </c>
       <c r="F38" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="5"/>
@@ -2342,21 +1935,21 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" s="1">
-        <f ca="1">TODAY() - 3</f>
-        <v>44097</v>
+        <f ca="1">TODAY() - 82</f>
+        <v>44091</v>
       </c>
       <c r="E39" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D39) / VLOOKUP(C39, tiers, 2, FALSE), "")</f>
-        <v>0.9732142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C39, tiers, 2, FALSE)), "", IF(ISBLANK(D39), -1, 1 - (TODAY() - D39) / VLOOKUP(C39, tiers, 2, FALSE)))</f>
+        <v>0.2678571428571429</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="5"/>
@@ -2366,21 +1959,21 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" s="1">
-        <f ca="1">TODAY() - 3</f>
-        <v>44097</v>
+        <f ca="1">TODAY() - 79</f>
+        <v>44094</v>
       </c>
       <c r="E40" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D40) / VLOOKUP(C40, tiers, 2, FALSE), "")</f>
-        <v>0.9732142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C40, tiers, 2, FALSE)), "", IF(ISBLANK(D40), -1, 1 - (TODAY() - D40) / VLOOKUP(C40, tiers, 2, FALSE)))</f>
+        <v>0.2946428571428571</v>
       </c>
       <c r="F40" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="5"/>
@@ -2390,21 +1983,21 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41">
+        <v>135</v>
+      </c>
+      <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="1">
-        <f ca="1">TODAY() - 3</f>
-        <v>44097</v>
+        <f ca="1">TODAY() - 78</f>
+        <v>44095</v>
       </c>
       <c r="E41" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D41) / VLOOKUP(C41, tiers, 2, FALSE), "")</f>
-        <v>0.9732142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C41, tiers, 2, FALSE)), "", IF(ISBLANK(D41), -1, 1 - (TODAY() - D41) / VLOOKUP(C41, tiers, 2, FALSE)))</f>
+        <v>0.3035714285714286</v>
       </c>
       <c r="F41" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="5"/>
@@ -2414,18 +2007,18 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" s="1">
-        <f ca="1">TODAY() - 4</f>
-        <v>44096</v>
+        <f ca="1">TODAY() - 75</f>
+        <v>44098</v>
       </c>
       <c r="E42" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D42) / VLOOKUP(C42, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C42, tiers, 2, FALSE)), "", IF(ISBLANK(D42), -1, 1 - (TODAY() - D42) / VLOOKUP(C42, tiers, 2, FALSE)))</f>
+        <v>0.3303571428571429</v>
       </c>
       <c r="F42" t="s">
         <v>38</v>
@@ -2438,21 +2031,21 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" s="1">
-        <f ca="1">TODAY() - 4</f>
-        <v>44096</v>
+        <f ca="1">TODAY() - 69</f>
+        <v>44104</v>
       </c>
       <c r="E43" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D43) / VLOOKUP(C43, tiers, 2, FALSE), "")</f>
-        <v>0.9642857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C43, tiers, 2, FALSE)), "", IF(ISBLANK(D43), -1, 1 - (TODAY() - D43) / VLOOKUP(C43, tiers, 2, FALSE)))</f>
+        <v>0.3839285714285714</v>
       </c>
       <c r="F43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="5"/>
@@ -2462,21 +2055,21 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" s="1">
-        <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <f ca="1">TODAY() - 68</f>
+        <v>44105</v>
       </c>
       <c r="E44" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D44) / VLOOKUP(C44, tiers, 2, FALSE), "")</f>
-        <v>0.9553571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C44, tiers, 2, FALSE)), "", IF(ISBLANK(D44), -1, 1 - (TODAY() - D44) / VLOOKUP(C44, tiers, 2, FALSE)))</f>
+        <v>0.3928571428571429</v>
       </c>
       <c r="F44" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="5"/>
@@ -2486,21 +2079,21 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <f ca="1">TODAY() - 66</f>
+        <v>44107</v>
       </c>
       <c r="E45" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D45) / VLOOKUP(C45, tiers, 2, FALSE), "")</f>
-        <v>0.9553571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C45, tiers, 2, FALSE)), "", IF(ISBLANK(D45), -1, 1 - (TODAY() - D45) / VLOOKUP(C45, tiers, 2, FALSE)))</f>
+        <v>0.4107142857142857</v>
       </c>
       <c r="F45" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="5"/>
@@ -2510,18 +2103,18 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" s="1">
-        <f ca="1">TODAY() - 5</f>
-        <v>44095</v>
+        <f ca="1">TODAY() - 62</f>
+        <v>44111</v>
       </c>
       <c r="E46" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D46) / VLOOKUP(C46, tiers, 2, FALSE), "")</f>
-        <v>0.9553571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C46, tiers, 2, FALSE)), "", IF(ISBLANK(D46), -1, 1 - (TODAY() - D46) / VLOOKUP(C46, tiers, 2, FALSE)))</f>
+        <v>0.4464285714285714</v>
       </c>
       <c r="F46" t="s">
         <v>37</v>
@@ -2534,21 +2127,21 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="2">
+        <v>11</v>
+      </c>
+      <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" s="1">
-        <f ca="1">TODAY() - 6</f>
-        <v>44094</v>
+        <f ca="1">TODAY() - 59</f>
+        <v>44114</v>
       </c>
       <c r="E47" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D47) / VLOOKUP(C47, tiers, 2, FALSE), "")</f>
-        <v>0.9464285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C47, tiers, 2, FALSE)), "", IF(ISBLANK(D47), -1, 1 - (TODAY() - D47) / VLOOKUP(C47, tiers, 2, FALSE)))</f>
+        <v>0.4732142857142857</v>
       </c>
       <c r="F47" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="5"/>
@@ -2558,21 +2151,21 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="2">
+        <v>119</v>
+      </c>
+      <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" s="1">
-        <f ca="1">TODAY() - 7</f>
-        <v>44093</v>
+        <f ca="1">TODAY() - 55</f>
+        <v>44118</v>
       </c>
       <c r="E48" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D48) / VLOOKUP(C48, tiers, 2, FALSE), "")</f>
-        <v>0.9375</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C48, tiers, 2, FALSE)), "", IF(ISBLANK(D48), -1, 1 - (TODAY() - D48) / VLOOKUP(C48, tiers, 2, FALSE)))</f>
+        <v>0.5089285714285714</v>
       </c>
       <c r="F48" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="5"/>
@@ -2582,21 +2175,21 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 53</f>
+        <v>44120</v>
       </c>
       <c r="E49" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D49) / VLOOKUP(C49, tiers, 2, FALSE), "")</f>
-        <v>0.9285714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C49, tiers, 2, FALSE)), "", IF(ISBLANK(D49), -1, 1 - (TODAY() - D49) / VLOOKUP(C49, tiers, 2, FALSE)))</f>
+        <v>0.5267857142857143</v>
       </c>
       <c r="F49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="5"/>
@@ -2606,18 +2199,18 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 48</f>
+        <v>44125</v>
       </c>
       <c r="E50" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D50) / VLOOKUP(C50, tiers, 2, FALSE), "")</f>
-        <v>0.9285714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C50, tiers, 2, FALSE)), "", IF(ISBLANK(D50), -1, 1 - (TODAY() - D50) / VLOOKUP(C50, tiers, 2, FALSE)))</f>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F50" t="s">
         <v>151</v>
@@ -2630,21 +2223,21 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 47</f>
+        <v>44126</v>
       </c>
       <c r="E51" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D51) / VLOOKUP(C51, tiers, 2, FALSE), "")</f>
-        <v>0.9285714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C51, tiers, 2, FALSE)), "", IF(ISBLANK(D51), -1, 1 - (TODAY() - D51) / VLOOKUP(C51, tiers, 2, FALSE)))</f>
+        <v>0.58035714285714279</v>
       </c>
       <c r="F51" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="5"/>
@@ -2654,21 +2247,21 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" s="1">
-        <f ca="1">TODAY() - 8</f>
-        <v>44092</v>
+        <f ca="1">TODAY() - 46</f>
+        <v>44127</v>
       </c>
       <c r="E52" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D52) / VLOOKUP(C52, tiers, 2, FALSE), "")</f>
-        <v>0.9285714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C52, tiers, 2, FALSE)), "", IF(ISBLANK(D52), -1, 1 - (TODAY() - D52) / VLOOKUP(C52, tiers, 2, FALSE)))</f>
+        <v>0.5892857142857143</v>
       </c>
       <c r="F52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="5"/>
@@ -2678,21 +2271,21 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" s="1">
-        <f ca="1">TODAY() - 9</f>
-        <v>44091</v>
+        <f ca="1">TODAY() - 46</f>
+        <v>44127</v>
       </c>
       <c r="E53" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D53) / VLOOKUP(C53, tiers, 2, FALSE), "")</f>
-        <v>0.9196428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C53, tiers, 2, FALSE)), "", IF(ISBLANK(D53), -1, 1 - (TODAY() - D53) / VLOOKUP(C53, tiers, 2, FALSE)))</f>
+        <v>0.5892857142857143</v>
       </c>
       <c r="F53" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="5"/>
@@ -2702,21 +2295,21 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" s="1">
-        <f ca="1">TODAY() - 9</f>
-        <v>44091</v>
+        <f ca="1">TODAY() - 45</f>
+        <v>44128</v>
       </c>
       <c r="E54" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D54) / VLOOKUP(C54, tiers, 2, FALSE), "")</f>
-        <v>0.9196428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C54, tiers, 2, FALSE)), "", IF(ISBLANK(D54), -1, 1 - (TODAY() - D54) / VLOOKUP(C54, tiers, 2, FALSE)))</f>
+        <v>0.5982142857142857</v>
       </c>
       <c r="F54" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="5"/>
@@ -2726,21 +2319,21 @@
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" s="1">
-        <f ca="1">TODAY() - 9</f>
-        <v>44091</v>
+        <f ca="1">TODAY() - 45</f>
+        <v>44128</v>
       </c>
       <c r="E55" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D55) / VLOOKUP(C55, tiers, 2, FALSE), "")</f>
-        <v>0.9196428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C55, tiers, 2, FALSE)), "", IF(ISBLANK(D55), -1, 1 - (TODAY() - D55) / VLOOKUP(C55, tiers, 2, FALSE)))</f>
+        <v>0.5982142857142857</v>
       </c>
       <c r="F55" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="5"/>
@@ -2750,21 +2343,21 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" s="1">
-        <f ca="1">TODAY() - 9</f>
-        <v>44091</v>
+        <f ca="1">TODAY() - 44</f>
+        <v>44129</v>
       </c>
       <c r="E56" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D56) / VLOOKUP(C56, tiers, 2, FALSE), "")</f>
-        <v>0.9196428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C56, tiers, 2, FALSE)), "", IF(ISBLANK(D56), -1, 1 - (TODAY() - D56) / VLOOKUP(C56, tiers, 2, FALSE)))</f>
+        <v>0.60714285714285721</v>
       </c>
       <c r="F56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="5"/>
@@ -2774,21 +2367,21 @@
         <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" s="1">
-        <f ca="1">TODAY() - 11</f>
-        <v>44089</v>
+        <f ca="1">TODAY() - 43</f>
+        <v>44130</v>
       </c>
       <c r="E57" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D57) / VLOOKUP(C57, tiers, 2, FALSE), "")</f>
-        <v>0.9017857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C57, tiers, 2, FALSE)), "", IF(ISBLANK(D57), -1, 1 - (TODAY() - D57) / VLOOKUP(C57, tiers, 2, FALSE)))</f>
+        <v>0.6160714285714286</v>
       </c>
       <c r="F57" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="5"/>
@@ -2798,21 +2391,21 @@
         <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" s="1">
-        <f ca="1">TODAY() - 11</f>
-        <v>44089</v>
+        <f ca="1">TODAY() - 43</f>
+        <v>44130</v>
       </c>
       <c r="E58" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D58) / VLOOKUP(C58, tiers, 2, FALSE), "")</f>
-        <v>0.9017857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C58, tiers, 2, FALSE)), "", IF(ISBLANK(D58), -1, 1 - (TODAY() - D58) / VLOOKUP(C58, tiers, 2, FALSE)))</f>
+        <v>0.6160714285714286</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="5"/>
@@ -2822,21 +2415,21 @@
         <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" s="1">
-        <f ca="1">TODAY() - 11</f>
-        <v>44089</v>
+        <f ca="1">TODAY() - 41</f>
+        <v>44132</v>
       </c>
       <c r="E59" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D59) / VLOOKUP(C59, tiers, 2, FALSE), "")</f>
-        <v>0.9017857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C59, tiers, 2, FALSE)), "", IF(ISBLANK(D59), -1, 1 - (TODAY() - D59) / VLOOKUP(C59, tiers, 2, FALSE)))</f>
+        <v>0.6339285714285714</v>
       </c>
       <c r="F59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="5"/>
@@ -2846,21 +2439,21 @@
         <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="2">
+        <v>138</v>
+      </c>
+      <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" s="1">
-        <f ca="1">TODAY() - 12</f>
-        <v>44088</v>
+        <f ca="1">TODAY() - 41</f>
+        <v>44132</v>
       </c>
       <c r="E60" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D60) / VLOOKUP(C60, tiers, 2, FALSE), "")</f>
-        <v>0.8928571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C60, tiers, 2, FALSE)), "", IF(ISBLANK(D60), -1, 1 - (TODAY() - D60) / VLOOKUP(C60, tiers, 2, FALSE)))</f>
+        <v>0.6339285714285714</v>
       </c>
       <c r="F60" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="5"/>
@@ -2870,21 +2463,21 @@
         <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" s="1">
-        <f ca="1">TODAY() - 12</f>
-        <v>44088</v>
+        <f ca="1">TODAY() - 40</f>
+        <v>44133</v>
       </c>
       <c r="E61" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D61) / VLOOKUP(C61, tiers, 2, FALSE), "")</f>
-        <v>0.8928571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C61, tiers, 2, FALSE)), "", IF(ISBLANK(D61), -1, 1 - (TODAY() - D61) / VLOOKUP(C61, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="5"/>
@@ -2894,21 +2487,21 @@
         <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" s="1">
-        <f ca="1">TODAY() - 13</f>
-        <v>44087</v>
+        <f ca="1">TODAY() - 40</f>
+        <v>44133</v>
       </c>
       <c r="E62" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D62) / VLOOKUP(C62, tiers, 2, FALSE), "")</f>
-        <v>0.8839285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C62, tiers, 2, FALSE)), "", IF(ISBLANK(D62), -1, 1 - (TODAY() - D62) / VLOOKUP(C62, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="5"/>
@@ -2918,21 +2511,21 @@
         <v>43</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" s="1">
-        <f ca="1">TODAY() - 13</f>
-        <v>44087</v>
+        <f ca="1">TODAY() - 40</f>
+        <v>44133</v>
       </c>
       <c r="E63" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D63) / VLOOKUP(C63, tiers, 2, FALSE), "")</f>
-        <v>0.8839285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C63, tiers, 2, FALSE)), "", IF(ISBLANK(D63), -1, 1 - (TODAY() - D63) / VLOOKUP(C63, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="5"/>
@@ -2942,21 +2535,21 @@
         <v>43</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" s="1">
-        <f ca="1">TODAY() - 13</f>
-        <v>44087</v>
+        <f ca="1">TODAY() - 40</f>
+        <v>44133</v>
       </c>
       <c r="E64" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D64) / VLOOKUP(C64, tiers, 2, FALSE), "")</f>
-        <v>0.8839285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C64, tiers, 2, FALSE)), "", IF(ISBLANK(D64), -1, 1 - (TODAY() - D64) / VLOOKUP(C64, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F64" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="5"/>
@@ -2966,21 +2559,21 @@
         <v>43</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" s="1">
-        <f ca="1">TODAY() - 14</f>
-        <v>44086</v>
+        <f ca="1">TODAY() - 40</f>
+        <v>44133</v>
       </c>
       <c r="E65" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D65) / VLOOKUP(C65, tiers, 2, FALSE), "")</f>
-        <v>0.875</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C65, tiers, 2, FALSE)), "", IF(ISBLANK(D65), -1, 1 - (TODAY() - D65) / VLOOKUP(C65, tiers, 2, FALSE)))</f>
+        <v>0.64285714285714279</v>
       </c>
       <c r="F65" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="5"/>
@@ -2990,21 +2583,21 @@
         <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" s="1">
-        <f ca="1">TODAY() - 15</f>
-        <v>44085</v>
+        <f ca="1">TODAY() - 39</f>
+        <v>44134</v>
       </c>
       <c r="E66" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D66) / VLOOKUP(C66, tiers, 2, FALSE), "")</f>
-        <v>0.8660714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C66, tiers, 2, FALSE)), "", IF(ISBLANK(D66), -1, 1 - (TODAY() - D66) / VLOOKUP(C66, tiers, 2, FALSE)))</f>
+        <v>0.6517857142857143</v>
       </c>
       <c r="F66" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="5"/>
@@ -3014,21 +2607,21 @@
         <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" s="1">
-        <f ca="1">TODAY() - 15</f>
-        <v>44085</v>
+        <f ca="1">TODAY() - 39</f>
+        <v>44134</v>
       </c>
       <c r="E67" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D67) / VLOOKUP(C67, tiers, 2, FALSE), "")</f>
-        <v>0.8660714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C67, tiers, 2, FALSE)), "", IF(ISBLANK(D67), -1, 1 - (TODAY() - D67) / VLOOKUP(C67, tiers, 2, FALSE)))</f>
+        <v>0.6517857142857143</v>
       </c>
       <c r="F67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="5"/>
@@ -3038,21 +2631,21 @@
         <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" s="1">
-        <f ca="1">TODAY() - 15</f>
-        <v>44085</v>
+        <f ca="1">TODAY() - 39</f>
+        <v>44134</v>
       </c>
       <c r="E68" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D68) / VLOOKUP(C68, tiers, 2, FALSE), "")</f>
-        <v>0.8660714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C68, tiers, 2, FALSE)), "", IF(ISBLANK(D68), -1, 1 - (TODAY() - D68) / VLOOKUP(C68, tiers, 2, FALSE)))</f>
+        <v>0.6517857142857143</v>
       </c>
       <c r="F68" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="5"/>
@@ -3062,21 +2655,21 @@
         <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" s="1">
-        <f ca="1">TODAY() - 15</f>
-        <v>44085</v>
+        <f ca="1">TODAY() - 38</f>
+        <v>44135</v>
       </c>
       <c r="E69" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D69) / VLOOKUP(C69, tiers, 2, FALSE), "")</f>
-        <v>0.8660714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C69, tiers, 2, FALSE)), "", IF(ISBLANK(D69), -1, 1 - (TODAY() - D69) / VLOOKUP(C69, tiers, 2, FALSE)))</f>
+        <v>0.6607142857142857</v>
       </c>
       <c r="F69" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="5"/>
@@ -3086,21 +2679,21 @@
         <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" s="1">
-        <f ca="1">TODAY() - 15</f>
-        <v>44085</v>
+        <f ca="1">TODAY() - 37</f>
+        <v>44136</v>
       </c>
       <c r="E70" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D70) / VLOOKUP(C70, tiers, 2, FALSE), "")</f>
-        <v>0.8660714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C70, tiers, 2, FALSE)), "", IF(ISBLANK(D70), -1, 1 - (TODAY() - D70) / VLOOKUP(C70, tiers, 2, FALSE)))</f>
+        <v>0.66964285714285721</v>
       </c>
       <c r="F70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="5"/>
@@ -3110,21 +2703,21 @@
         <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" s="1">
-        <f ca="1">TODAY() - 16</f>
-        <v>44084</v>
+        <f ca="1">TODAY() - 37</f>
+        <v>44136</v>
       </c>
       <c r="E71" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D71) / VLOOKUP(C71, tiers, 2, FALSE), "")</f>
-        <v>0.85714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C71, tiers, 2, FALSE)), "", IF(ISBLANK(D71), -1, 1 - (TODAY() - D71) / VLOOKUP(C71, tiers, 2, FALSE)))</f>
+        <v>0.66964285714285721</v>
       </c>
       <c r="F71" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="5"/>
@@ -3134,21 +2727,21 @@
         <v>43</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" s="1">
-        <f ca="1">TODAY() - 16</f>
-        <v>44084</v>
+        <f ca="1">TODAY() - 36</f>
+        <v>44137</v>
       </c>
       <c r="E72" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D72) / VLOOKUP(C72, tiers, 2, FALSE), "")</f>
-        <v>0.85714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C72, tiers, 2, FALSE)), "", IF(ISBLANK(D72), -1, 1 - (TODAY() - D72) / VLOOKUP(C72, tiers, 2, FALSE)))</f>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F72" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="5"/>
@@ -3158,21 +2751,21 @@
         <v>43</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73">
+        <v>114</v>
+      </c>
+      <c r="C73" s="2">
         <v>1</v>
       </c>
       <c r="D73" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 36</f>
+        <v>44137</v>
       </c>
       <c r="E73" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D73) / VLOOKUP(C73, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C73, tiers, 2, FALSE)), "", IF(ISBLANK(D73), -1, 1 - (TODAY() - D73) / VLOOKUP(C73, tiers, 2, FALSE)))</f>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F73" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" s="5"/>
@@ -3182,21 +2775,21 @@
         <v>43</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 34</f>
+        <v>44139</v>
       </c>
       <c r="E74" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D74) / VLOOKUP(C74, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C74, tiers, 2, FALSE)), "", IF(ISBLANK(D74), -1, 1 - (TODAY() - D74) / VLOOKUP(C74, tiers, 2, FALSE)))</f>
+        <v>0.6964285714285714</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="5"/>
@@ -3206,21 +2799,21 @@
         <v>43</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
-      </c>
-      <c r="C75" s="2">
+        <v>128</v>
+      </c>
+      <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 34</f>
+        <v>44139</v>
       </c>
       <c r="E75" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D75) / VLOOKUP(C75, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C75, tiers, 2, FALSE)), "", IF(ISBLANK(D75), -1, 1 - (TODAY() - D75) / VLOOKUP(C75, tiers, 2, FALSE)))</f>
+        <v>0.6964285714285714</v>
       </c>
       <c r="F75" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="5"/>
@@ -3230,21 +2823,21 @@
         <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 34</f>
+        <v>44139</v>
       </c>
       <c r="E76" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D76) / VLOOKUP(C76, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C76, tiers, 2, FALSE)), "", IF(ISBLANK(D76), -1, 1 - (TODAY() - D76) / VLOOKUP(C76, tiers, 2, FALSE)))</f>
+        <v>0.6964285714285714</v>
       </c>
       <c r="F76" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="G76" s="1"/>
       <c r="H76" s="5"/>
@@ -3254,21 +2847,21 @@
         <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 34</f>
+        <v>44139</v>
       </c>
       <c r="E77" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D77) / VLOOKUP(C77, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C77, tiers, 2, FALSE)), "", IF(ISBLANK(D77), -1, 1 - (TODAY() - D77) / VLOOKUP(C77, tiers, 2, FALSE)))</f>
+        <v>0.6964285714285714</v>
       </c>
       <c r="F77" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="5"/>
@@ -3278,21 +2871,21 @@
         <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" s="1">
-        <f ca="1">TODAY() - 18</f>
-        <v>44082</v>
+        <f ca="1">TODAY() - 34</f>
+        <v>44139</v>
       </c>
       <c r="E78" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D78) / VLOOKUP(C78, tiers, 2, FALSE), "")</f>
-        <v>0.8392857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C78, tiers, 2, FALSE)), "", IF(ISBLANK(D78), -1, 1 - (TODAY() - D78) / VLOOKUP(C78, tiers, 2, FALSE)))</f>
+        <v>0.6964285714285714</v>
       </c>
       <c r="F78" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="5"/>
@@ -3302,21 +2895,21 @@
         <v>43</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" s="1">
-        <f ca="1">TODAY() - 19</f>
-        <v>44081</v>
+        <f ca="1">TODAY() - 33</f>
+        <v>44140</v>
       </c>
       <c r="E79" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D79) / VLOOKUP(C79, tiers, 2, FALSE), "")</f>
-        <v>0.83035714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C79, tiers, 2, FALSE)), "", IF(ISBLANK(D79), -1, 1 - (TODAY() - D79) / VLOOKUP(C79, tiers, 2, FALSE)))</f>
+        <v>0.70535714285714279</v>
       </c>
       <c r="F79" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="5"/>
@@ -3326,21 +2919,21 @@
         <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" s="1">
-        <f ca="1">TODAY() - 19</f>
-        <v>44081</v>
+        <f ca="1">TODAY() - 33</f>
+        <v>44140</v>
       </c>
       <c r="E80" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D80) / VLOOKUP(C80, tiers, 2, FALSE), "")</f>
-        <v>0.83035714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C80, tiers, 2, FALSE)), "", IF(ISBLANK(D80), -1, 1 - (TODAY() - D80) / VLOOKUP(C80, tiers, 2, FALSE)))</f>
+        <v>0.70535714285714279</v>
       </c>
       <c r="F80" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="5"/>
@@ -3350,21 +2943,21 @@
         <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>62</v>
-      </c>
-      <c r="C81" s="2">
+        <v>126</v>
+      </c>
+      <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" s="1">
-        <f ca="1">TODAY() - 19</f>
-        <v>44081</v>
+        <f ca="1">TODAY() - 32</f>
+        <v>44141</v>
       </c>
       <c r="E81" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D81) / VLOOKUP(C81, tiers, 2, FALSE), "")</f>
-        <v>0.83035714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C81, tiers, 2, FALSE)), "", IF(ISBLANK(D81), -1, 1 - (TODAY() - D81) / VLOOKUP(C81, tiers, 2, FALSE)))</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F81" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="5"/>
@@ -3374,21 +2967,21 @@
         <v>43</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" s="1">
-        <f ca="1">TODAY() - 19</f>
-        <v>44081</v>
+        <f ca="1">TODAY() - 31</f>
+        <v>44142</v>
       </c>
       <c r="E82" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D82) / VLOOKUP(C82, tiers, 2, FALSE), "")</f>
-        <v>0.83035714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C82, tiers, 2, FALSE)), "", IF(ISBLANK(D82), -1, 1 - (TODAY() - D82) / VLOOKUP(C82, tiers, 2, FALSE)))</f>
+        <v>0.7232142857142857</v>
       </c>
       <c r="F82" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="5"/>
@@ -3398,18 +2991,18 @@
         <v>43</v>
       </c>
       <c r="B83" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" s="1">
-        <f ca="1">TODAY() - 20</f>
-        <v>44080</v>
+        <f ca="1">TODAY() - 31</f>
+        <v>44142</v>
       </c>
       <c r="E83" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D83) / VLOOKUP(C83, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C83, tiers, 2, FALSE)), "", IF(ISBLANK(D83), -1, 1 - (TODAY() - D83) / VLOOKUP(C83, tiers, 2, FALSE)))</f>
+        <v>0.7232142857142857</v>
       </c>
       <c r="F83" t="s">
         <v>39</v>
@@ -3422,18 +3015,18 @@
         <v>43</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" s="1">
-        <f ca="1">TODAY() - 20</f>
-        <v>44080</v>
+        <f ca="1">TODAY() - 31</f>
+        <v>44142</v>
       </c>
       <c r="E84" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D84) / VLOOKUP(C84, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C84, tiers, 2, FALSE)), "", IF(ISBLANK(D84), -1, 1 - (TODAY() - D84) / VLOOKUP(C84, tiers, 2, FALSE)))</f>
+        <v>0.7232142857142857</v>
       </c>
       <c r="F84" t="s">
         <v>34</v>
@@ -3446,21 +3039,21 @@
         <v>43</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85" s="1">
-        <f ca="1">TODAY() - 20</f>
-        <v>44080</v>
+        <f ca="1">TODAY() - 30</f>
+        <v>44143</v>
       </c>
       <c r="E85" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D85) / VLOOKUP(C85, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C85, tiers, 2, FALSE)), "", IF(ISBLANK(D85), -1, 1 - (TODAY() - D85) / VLOOKUP(C85, tiers, 2, FALSE)))</f>
+        <v>0.73214285714285721</v>
       </c>
       <c r="F85" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G85" s="1"/>
       <c r="H85" s="5"/>
@@ -3470,21 +3063,21 @@
         <v>43</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86" s="1">
-        <f ca="1">TODAY() - 20</f>
-        <v>44080</v>
+        <f ca="1">TODAY() - 30</f>
+        <v>44143</v>
       </c>
       <c r="E86" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D86) / VLOOKUP(C86, tiers, 2, FALSE), "")</f>
-        <v>0.8214285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C86, tiers, 2, FALSE)), "", IF(ISBLANK(D86), -1, 1 - (TODAY() - D86) / VLOOKUP(C86, tiers, 2, FALSE)))</f>
+        <v>0.73214285714285721</v>
       </c>
       <c r="F86" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="5"/>
@@ -3494,21 +3087,21 @@
         <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" s="1">
-        <f ca="1">TODAY() - 21</f>
-        <v>44079</v>
+        <f ca="1">TODAY() - 30</f>
+        <v>44143</v>
       </c>
       <c r="E87" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D87) / VLOOKUP(C87, tiers, 2, FALSE), "")</f>
-        <v>0.8125</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C87, tiers, 2, FALSE)), "", IF(ISBLANK(D87), -1, 1 - (TODAY() - D87) / VLOOKUP(C87, tiers, 2, FALSE)))</f>
+        <v>0.73214285714285721</v>
       </c>
       <c r="F87" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="5"/>
@@ -3518,21 +3111,21 @@
         <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" s="1">
-        <f ca="1">TODAY() - 22</f>
-        <v>44078</v>
+        <f ca="1">TODAY() - 29</f>
+        <v>44144</v>
       </c>
       <c r="E88" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D88) / VLOOKUP(C88, tiers, 2, FALSE), "")</f>
-        <v>0.8035714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C88, tiers, 2, FALSE)), "", IF(ISBLANK(D88), -1, 1 - (TODAY() - D88) / VLOOKUP(C88, tiers, 2, FALSE)))</f>
+        <v>0.7410714285714286</v>
       </c>
       <c r="F88" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="5"/>
@@ -3542,21 +3135,21 @@
         <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" s="1">
-        <f ca="1">TODAY() - 22</f>
-        <v>44078</v>
+        <f ca="1">TODAY() - 28</f>
+        <v>44145</v>
       </c>
       <c r="E89" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D89) / VLOOKUP(C89, tiers, 2, FALSE), "")</f>
-        <v>0.8035714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C89, tiers, 2, FALSE)), "", IF(ISBLANK(D89), -1, 1 - (TODAY() - D89) / VLOOKUP(C89, tiers, 2, FALSE)))</f>
+        <v>0.75</v>
       </c>
       <c r="F89" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="5"/>
@@ -3566,21 +3159,21 @@
         <v>43</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" s="1">
-        <f ca="1">TODAY() - 22</f>
-        <v>44078</v>
+        <f ca="1">TODAY() - 25</f>
+        <v>44148</v>
       </c>
       <c r="E90" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D90) / VLOOKUP(C90, tiers, 2, FALSE), "")</f>
-        <v>0.8035714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C90, tiers, 2, FALSE)), "", IF(ISBLANK(D90), -1, 1 - (TODAY() - D90) / VLOOKUP(C90, tiers, 2, FALSE)))</f>
+        <v>0.7767857142857143</v>
       </c>
       <c r="F90" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="5"/>
@@ -3590,21 +3183,21 @@
         <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" s="1">
-        <f ca="1">TODAY() - 22</f>
-        <v>44078</v>
+        <f ca="1">TODAY() - 23</f>
+        <v>44150</v>
       </c>
       <c r="E91" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D91) / VLOOKUP(C91, tiers, 2, FALSE), "")</f>
-        <v>0.8035714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C91, tiers, 2, FALSE)), "", IF(ISBLANK(D91), -1, 1 - (TODAY() - D91) / VLOOKUP(C91, tiers, 2, FALSE)))</f>
+        <v>0.79464285714285721</v>
       </c>
       <c r="F91" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="5"/>
@@ -3614,21 +3207,21 @@
         <v>43</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" s="1">
-        <f ca="1">TODAY() - 23</f>
-        <v>44077</v>
+        <f ca="1">TODAY() - 22</f>
+        <v>44151</v>
       </c>
       <c r="E92" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D92) / VLOOKUP(C92, tiers, 2, FALSE), "")</f>
-        <v>0.79464285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C92, tiers, 2, FALSE)), "", IF(ISBLANK(D92), -1, 1 - (TODAY() - D92) / VLOOKUP(C92, tiers, 2, FALSE)))</f>
+        <v>0.8035714285714286</v>
       </c>
       <c r="F92" t="s">
-        <v>38</v>
+        <v>150</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="5"/>
@@ -3638,21 +3231,21 @@
         <v>43</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93" s="1">
-        <f ca="1">TODAY() - 25</f>
-        <v>44075</v>
+        <f ca="1">TODAY() - 22</f>
+        <v>44151</v>
       </c>
       <c r="E93" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D93) / VLOOKUP(C93, tiers, 2, FALSE), "")</f>
-        <v>0.7767857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C93, tiers, 2, FALSE)), "", IF(ISBLANK(D93), -1, 1 - (TODAY() - D93) / VLOOKUP(C93, tiers, 2, FALSE)))</f>
+        <v>0.8035714285714286</v>
       </c>
       <c r="F93" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="5"/>
@@ -3662,21 +3255,21 @@
         <v>43</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94" s="1">
-        <f ca="1">TODAY() - 28</f>
-        <v>44072</v>
+        <f ca="1">TODAY() - 22</f>
+        <v>44151</v>
       </c>
       <c r="E94" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D94) / VLOOKUP(C94, tiers, 2, FALSE), "")</f>
-        <v>0.75</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C94, tiers, 2, FALSE)), "", IF(ISBLANK(D94), -1, 1 - (TODAY() - D94) / VLOOKUP(C94, tiers, 2, FALSE)))</f>
+        <v>0.8035714285714286</v>
       </c>
       <c r="F94" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G94" s="1"/>
       <c r="H94" s="5"/>
@@ -3686,21 +3279,21 @@
         <v>43</v>
       </c>
       <c r="B95" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95" s="1">
-        <f ca="1">TODAY() - 29</f>
-        <v>44071</v>
+        <f ca="1">TODAY() - 22</f>
+        <v>44151</v>
       </c>
       <c r="E95" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D95) / VLOOKUP(C95, tiers, 2, FALSE), "")</f>
-        <v>0.7410714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C95, tiers, 2, FALSE)), "", IF(ISBLANK(D95), -1, 1 - (TODAY() - D95) / VLOOKUP(C95, tiers, 2, FALSE)))</f>
+        <v>0.8035714285714286</v>
       </c>
       <c r="F95" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="5"/>
@@ -3710,21 +3303,21 @@
         <v>43</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96" s="1">
-        <f ca="1">TODAY() - 30</f>
-        <v>44070</v>
+        <f ca="1">TODAY() - 21</f>
+        <v>44152</v>
       </c>
       <c r="E96" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D96) / VLOOKUP(C96, tiers, 2, FALSE), "")</f>
-        <v>0.73214285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C96, tiers, 2, FALSE)), "", IF(ISBLANK(D96), -1, 1 - (TODAY() - D96) / VLOOKUP(C96, tiers, 2, FALSE)))</f>
+        <v>0.8125</v>
       </c>
       <c r="F96" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="5"/>
@@ -3734,21 +3327,21 @@
         <v>43</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97" s="1">
-        <f ca="1">TODAY() - 30</f>
-        <v>44070</v>
+        <f ca="1">TODAY() - 20</f>
+        <v>44153</v>
       </c>
       <c r="E97" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D97) / VLOOKUP(C97, tiers, 2, FALSE), "")</f>
-        <v>0.73214285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C97, tiers, 2, FALSE)), "", IF(ISBLANK(D97), -1, 1 - (TODAY() - D97) / VLOOKUP(C97, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F97" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G97" s="1"/>
       <c r="H97" s="5"/>
@@ -3758,21 +3351,21 @@
         <v>43</v>
       </c>
       <c r="B98" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98" s="1">
-        <f ca="1">TODAY() - 30</f>
-        <v>44070</v>
+        <f ca="1">TODAY() - 20</f>
+        <v>44153</v>
       </c>
       <c r="E98" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D98) / VLOOKUP(C98, tiers, 2, FALSE), "")</f>
-        <v>0.73214285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C98, tiers, 2, FALSE)), "", IF(ISBLANK(D98), -1, 1 - (TODAY() - D98) / VLOOKUP(C98, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="5"/>
@@ -3782,21 +3375,21 @@
         <v>43</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" s="1">
-        <f ca="1">TODAY() - 31</f>
-        <v>44069</v>
+        <f ca="1">TODAY() - 20</f>
+        <v>44153</v>
       </c>
       <c r="E99" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D99) / VLOOKUP(C99, tiers, 2, FALSE), "")</f>
-        <v>0.7232142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C99, tiers, 2, FALSE)), "", IF(ISBLANK(D99), -1, 1 - (TODAY() - D99) / VLOOKUP(C99, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F99" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="5"/>
@@ -3806,21 +3399,21 @@
         <v>43</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100" s="1">
-        <f ca="1">TODAY() - 31</f>
-        <v>44069</v>
+        <f ca="1">TODAY() - 20</f>
+        <v>44153</v>
       </c>
       <c r="E100" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D100) / VLOOKUP(C100, tiers, 2, FALSE), "")</f>
-        <v>0.7232142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C100, tiers, 2, FALSE)), "", IF(ISBLANK(D100), -1, 1 - (TODAY() - D100) / VLOOKUP(C100, tiers, 2, FALSE)))</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F100" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" s="5"/>
@@ -3830,21 +3423,21 @@
         <v>43</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" s="1">
-        <f ca="1">TODAY() - 31</f>
-        <v>44069</v>
+        <f ca="1">TODAY() - 19</f>
+        <v>44154</v>
       </c>
       <c r="E101" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D101) / VLOOKUP(C101, tiers, 2, FALSE), "")</f>
-        <v>0.7232142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C101, tiers, 2, FALSE)), "", IF(ISBLANK(D101), -1, 1 - (TODAY() - D101) / VLOOKUP(C101, tiers, 2, FALSE)))</f>
+        <v>0.83035714285714279</v>
       </c>
       <c r="F101" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="5"/>
@@ -3854,21 +3447,21 @@
         <v>43</v>
       </c>
       <c r="B102" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102" s="1">
-        <f ca="1">TODAY() - 32</f>
-        <v>44068</v>
+        <f ca="1">TODAY() - 19</f>
+        <v>44154</v>
       </c>
       <c r="E102" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D102) / VLOOKUP(C102, tiers, 2, FALSE), "")</f>
-        <v>0.7142857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C102, tiers, 2, FALSE)), "", IF(ISBLANK(D102), -1, 1 - (TODAY() - D102) / VLOOKUP(C102, tiers, 2, FALSE)))</f>
+        <v>0.83035714285714279</v>
       </c>
       <c r="F102" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="5"/>
@@ -3878,21 +3471,21 @@
         <v>43</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103">
+        <v>62</v>
+      </c>
+      <c r="C103" s="2">
         <v>1</v>
       </c>
       <c r="D103" s="1">
-        <f ca="1">TODAY() - 33</f>
-        <v>44067</v>
+        <f ca="1">TODAY() - 19</f>
+        <v>44154</v>
       </c>
       <c r="E103" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D103) / VLOOKUP(C103, tiers, 2, FALSE), "")</f>
-        <v>0.70535714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C103, tiers, 2, FALSE)), "", IF(ISBLANK(D103), -1, 1 - (TODAY() - D103) / VLOOKUP(C103, tiers, 2, FALSE)))</f>
+        <v>0.83035714285714279</v>
       </c>
       <c r="F103" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="5"/>
@@ -3902,21 +3495,21 @@
         <v>43</v>
       </c>
       <c r="B104" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104" s="1">
-        <f ca="1">TODAY() - 33</f>
-        <v>44067</v>
+        <f ca="1">TODAY() - 19</f>
+        <v>44154</v>
       </c>
       <c r="E104" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D104) / VLOOKUP(C104, tiers, 2, FALSE), "")</f>
-        <v>0.70535714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C104, tiers, 2, FALSE)), "", IF(ISBLANK(D104), -1, 1 - (TODAY() - D104) / VLOOKUP(C104, tiers, 2, FALSE)))</f>
+        <v>0.83035714285714279</v>
       </c>
       <c r="F104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="5"/>
@@ -3926,21 +3519,21 @@
         <v>43</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" s="1">
-        <f ca="1">TODAY() - 34</f>
-        <v>44066</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E105" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D105) / VLOOKUP(C105, tiers, 2, FALSE), "")</f>
-        <v>0.6964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C105, tiers, 2, FALSE)), "", IF(ISBLANK(D105), -1, 1 - (TODAY() - D105) / VLOOKUP(C105, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F105" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="5"/>
@@ -3950,21 +3543,21 @@
         <v>43</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" s="1">
-        <f ca="1">TODAY() - 34</f>
-        <v>44066</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E106" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D106) / VLOOKUP(C106, tiers, 2, FALSE), "")</f>
-        <v>0.6964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C106, tiers, 2, FALSE)), "", IF(ISBLANK(D106), -1, 1 - (TODAY() - D106) / VLOOKUP(C106, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F106" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" s="5"/>
@@ -3974,21 +3567,21 @@
         <v>43</v>
       </c>
       <c r="B107" t="s">
-        <v>129</v>
-      </c>
-      <c r="C107">
+        <v>96</v>
+      </c>
+      <c r="C107" s="2">
         <v>1</v>
       </c>
       <c r="D107" s="1">
-        <f ca="1">TODAY() - 34</f>
-        <v>44066</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E107" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D107) / VLOOKUP(C107, tiers, 2, FALSE), "")</f>
-        <v>0.6964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C107, tiers, 2, FALSE)), "", IF(ISBLANK(D107), -1, 1 - (TODAY() - D107) / VLOOKUP(C107, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F107" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" s="5"/>
@@ -3998,18 +3591,18 @@
         <v>43</v>
       </c>
       <c r="B108" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" s="1">
-        <f ca="1">TODAY() - 34</f>
-        <v>44066</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E108" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D108) / VLOOKUP(C108, tiers, 2, FALSE), "")</f>
-        <v>0.6964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C108, tiers, 2, FALSE)), "", IF(ISBLANK(D108), -1, 1 - (TODAY() - D108) / VLOOKUP(C108, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F108" t="s">
         <v>37</v>
@@ -4022,21 +3615,21 @@
         <v>43</v>
       </c>
       <c r="B109" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109" s="1">
-        <f ca="1">TODAY() - 34</f>
-        <v>44066</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E109" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D109) / VLOOKUP(C109, tiers, 2, FALSE), "")</f>
-        <v>0.6964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C109, tiers, 2, FALSE)), "", IF(ISBLANK(D109), -1, 1 - (TODAY() - D109) / VLOOKUP(C109, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F109" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" s="5"/>
@@ -4046,21 +3639,21 @@
         <v>43</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" s="1">
-        <f ca="1">TODAY() - 36</f>
-        <v>44064</v>
+        <f ca="1">TODAY() - 18</f>
+        <v>44155</v>
       </c>
       <c r="E110" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D110) / VLOOKUP(C110, tiers, 2, FALSE), "")</f>
-        <v>0.6785714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C110, tiers, 2, FALSE)), "", IF(ISBLANK(D110), -1, 1 - (TODAY() - D110) / VLOOKUP(C110, tiers, 2, FALSE)))</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="F110" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="G110" s="1"/>
       <c r="H110" s="5"/>
@@ -4070,21 +3663,21 @@
         <v>43</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
-      </c>
-      <c r="C111" s="2">
+        <v>16</v>
+      </c>
+      <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" s="1">
-        <f ca="1">TODAY() - 36</f>
-        <v>44064</v>
+        <f ca="1">TODAY() - 16</f>
+        <v>44157</v>
       </c>
       <c r="E111" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D111) / VLOOKUP(C111, tiers, 2, FALSE), "")</f>
-        <v>0.6785714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C111, tiers, 2, FALSE)), "", IF(ISBLANK(D111), -1, 1 - (TODAY() - D111) / VLOOKUP(C111, tiers, 2, FALSE)))</f>
+        <v>0.85714285714285721</v>
       </c>
       <c r="F111" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="5"/>
@@ -4094,21 +3687,21 @@
         <v>43</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" s="1">
-        <f ca="1">TODAY() - 37</f>
-        <v>44063</v>
+        <f ca="1">TODAY() - 16</f>
+        <v>44157</v>
       </c>
       <c r="E112" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D112) / VLOOKUP(C112, tiers, 2, FALSE), "")</f>
-        <v>0.66964285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C112, tiers, 2, FALSE)), "", IF(ISBLANK(D112), -1, 1 - (TODAY() - D112) / VLOOKUP(C112, tiers, 2, FALSE)))</f>
+        <v>0.85714285714285721</v>
       </c>
       <c r="F112" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="G112" s="1"/>
       <c r="H112" s="5"/>
@@ -4118,21 +3711,21 @@
         <v>43</v>
       </c>
       <c r="B113" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" s="1">
-        <f ca="1">TODAY() - 37</f>
-        <v>44063</v>
+        <f ca="1">TODAY() - 15</f>
+        <v>44158</v>
       </c>
       <c r="E113" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D113) / VLOOKUP(C113, tiers, 2, FALSE), "")</f>
-        <v>0.66964285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C113, tiers, 2, FALSE)), "", IF(ISBLANK(D113), -1, 1 - (TODAY() - D113) / VLOOKUP(C113, tiers, 2, FALSE)))</f>
+        <v>0.8660714285714286</v>
       </c>
       <c r="F113" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G113" s="1"/>
       <c r="H113" s="5"/>
@@ -4142,21 +3735,21 @@
         <v>43</v>
       </c>
       <c r="B114" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114" s="1">
-        <f ca="1">TODAY() - 38</f>
-        <v>44062</v>
+        <f ca="1">TODAY() - 15</f>
+        <v>44158</v>
       </c>
       <c r="E114" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D114) / VLOOKUP(C114, tiers, 2, FALSE), "")</f>
-        <v>0.6607142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C114, tiers, 2, FALSE)), "", IF(ISBLANK(D114), -1, 1 - (TODAY() - D114) / VLOOKUP(C114, tiers, 2, FALSE)))</f>
+        <v>0.8660714285714286</v>
       </c>
       <c r="F114" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G114" s="1"/>
       <c r="H114" s="5"/>
@@ -4166,21 +3759,21 @@
         <v>43</v>
       </c>
       <c r="B115" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115" s="1">
-        <f ca="1">TODAY() - 39</f>
-        <v>44061</v>
+        <f ca="1">TODAY() - 15</f>
+        <v>44158</v>
       </c>
       <c r="E115" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D115) / VLOOKUP(C115, tiers, 2, FALSE), "")</f>
-        <v>0.6517857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C115, tiers, 2, FALSE)), "", IF(ISBLANK(D115), -1, 1 - (TODAY() - D115) / VLOOKUP(C115, tiers, 2, FALSE)))</f>
+        <v>0.8660714285714286</v>
       </c>
       <c r="F115" t="s">
-        <v>38</v>
+        <v>150</v>
       </c>
       <c r="G115" s="1"/>
       <c r="H115" s="5"/>
@@ -4190,18 +3783,18 @@
         <v>43</v>
       </c>
       <c r="B116" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116" s="1">
-        <f ca="1">TODAY() - 39</f>
-        <v>44061</v>
+        <f ca="1">TODAY() - 15</f>
+        <v>44158</v>
       </c>
       <c r="E116" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D116) / VLOOKUP(C116, tiers, 2, FALSE), "")</f>
-        <v>0.6517857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C116, tiers, 2, FALSE)), "", IF(ISBLANK(D116), -1, 1 - (TODAY() - D116) / VLOOKUP(C116, tiers, 2, FALSE)))</f>
+        <v>0.8660714285714286</v>
       </c>
       <c r="F116" t="s">
         <v>37</v>
@@ -4214,21 +3807,21 @@
         <v>43</v>
       </c>
       <c r="B117" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117" s="1">
-        <f ca="1">TODAY() - 39</f>
-        <v>44061</v>
+        <f ca="1">TODAY() - 15</f>
+        <v>44158</v>
       </c>
       <c r="E117" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D117) / VLOOKUP(C117, tiers, 2, FALSE), "")</f>
-        <v>0.6517857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C117, tiers, 2, FALSE)), "", IF(ISBLANK(D117), -1, 1 - (TODAY() - D117) / VLOOKUP(C117, tiers, 2, FALSE)))</f>
+        <v>0.8660714285714286</v>
       </c>
       <c r="F117" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="5"/>
@@ -4238,21 +3831,21 @@
         <v>43</v>
       </c>
       <c r="B118" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118" s="1">
-        <f ca="1">TODAY() - 40</f>
-        <v>44060</v>
+        <f ca="1">TODAY() - 14</f>
+        <v>44159</v>
       </c>
       <c r="E118" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D118) / VLOOKUP(C118, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C118, tiers, 2, FALSE)), "", IF(ISBLANK(D118), -1, 1 - (TODAY() - D118) / VLOOKUP(C118, tiers, 2, FALSE)))</f>
+        <v>0.875</v>
       </c>
       <c r="F118" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G118" s="1"/>
       <c r="H118" s="5"/>
@@ -4262,21 +3855,21 @@
         <v>43</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119" s="1">
-        <f ca="1">TODAY() - 40</f>
-        <v>44060</v>
+        <f ca="1">TODAY() - 13</f>
+        <v>44160</v>
       </c>
       <c r="E119" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D119) / VLOOKUP(C119, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C119, tiers, 2, FALSE)), "", IF(ISBLANK(D119), -1, 1 - (TODAY() - D119) / VLOOKUP(C119, tiers, 2, FALSE)))</f>
+        <v>0.8839285714285714</v>
       </c>
       <c r="F119" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G119" s="1"/>
       <c r="H119" s="5"/>
@@ -4286,21 +3879,21 @@
         <v>43</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
+        <v>2</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120" s="1">
-        <f ca="1">TODAY() - 40</f>
-        <v>44060</v>
+        <f ca="1">TODAY() - 13</f>
+        <v>44160</v>
       </c>
       <c r="E120" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D120) / VLOOKUP(C120, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C120, tiers, 2, FALSE)), "", IF(ISBLANK(D120), -1, 1 - (TODAY() - D120) / VLOOKUP(C120, tiers, 2, FALSE)))</f>
+        <v>0.8839285714285714</v>
       </c>
       <c r="F120" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G120" s="1"/>
       <c r="H120" s="5"/>
@@ -4310,21 +3903,21 @@
         <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121" s="1">
-        <f ca="1">TODAY() - 40</f>
-        <v>44060</v>
+        <f ca="1">TODAY() - 13</f>
+        <v>44160</v>
       </c>
       <c r="E121" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D121) / VLOOKUP(C121, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C121, tiers, 2, FALSE)), "", IF(ISBLANK(D121), -1, 1 - (TODAY() - D121) / VLOOKUP(C121, tiers, 2, FALSE)))</f>
+        <v>0.8839285714285714</v>
       </c>
       <c r="F121" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="G121" s="1"/>
       <c r="H121" s="5"/>
@@ -4334,21 +3927,21 @@
         <v>43</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
-      </c>
-      <c r="C122">
+        <v>86</v>
+      </c>
+      <c r="C122" s="2">
         <v>1</v>
       </c>
       <c r="D122" s="1">
-        <f ca="1">TODAY() - 40</f>
-        <v>44060</v>
+        <f ca="1">TODAY() - 12</f>
+        <v>44161</v>
       </c>
       <c r="E122" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D122) / VLOOKUP(C122, tiers, 2, FALSE), "")</f>
-        <v>0.64285714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C122, tiers, 2, FALSE)), "", IF(ISBLANK(D122), -1, 1 - (TODAY() - D122) / VLOOKUP(C122, tiers, 2, FALSE)))</f>
+        <v>0.8928571428571429</v>
       </c>
       <c r="F122" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="5"/>
@@ -4358,21 +3951,21 @@
         <v>43</v>
       </c>
       <c r="B123" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123" s="1">
-        <f ca="1">TODAY() - 41</f>
-        <v>44059</v>
+        <f ca="1">TODAY() - 12</f>
+        <v>44161</v>
       </c>
       <c r="E123" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D123) / VLOOKUP(C123, tiers, 2, FALSE), "")</f>
-        <v>0.6339285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C123, tiers, 2, FALSE)), "", IF(ISBLANK(D123), -1, 1 - (TODAY() - D123) / VLOOKUP(C123, tiers, 2, FALSE)))</f>
+        <v>0.8928571428571429</v>
       </c>
       <c r="F123" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="5"/>
@@ -4382,21 +3975,21 @@
         <v>43</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" s="1">
-        <f ca="1">TODAY() - 41</f>
-        <v>44059</v>
+        <f ca="1">TODAY() - 11</f>
+        <v>44162</v>
       </c>
       <c r="E124" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D124) / VLOOKUP(C124, tiers, 2, FALSE), "")</f>
-        <v>0.6339285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C124, tiers, 2, FALSE)), "", IF(ISBLANK(D124), -1, 1 - (TODAY() - D124) / VLOOKUP(C124, tiers, 2, FALSE)))</f>
+        <v>0.9017857142857143</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="5"/>
@@ -4406,21 +3999,21 @@
         <v>43</v>
       </c>
       <c r="B125" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" s="1">
-        <f ca="1">TODAY() - 43</f>
-        <v>44057</v>
+        <f ca="1">TODAY() - 11</f>
+        <v>44162</v>
       </c>
       <c r="E125" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D125) / VLOOKUP(C125, tiers, 2, FALSE), "")</f>
-        <v>0.6160714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C125, tiers, 2, FALSE)), "", IF(ISBLANK(D125), -1, 1 - (TODAY() - D125) / VLOOKUP(C125, tiers, 2, FALSE)))</f>
+        <v>0.9017857142857143</v>
       </c>
       <c r="F125" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="5"/>
@@ -4430,21 +4023,21 @@
         <v>43</v>
       </c>
       <c r="B126" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126" s="1">
-        <f ca="1">TODAY() - 43</f>
-        <v>44057</v>
+        <f ca="1">TODAY() - 11</f>
+        <v>44162</v>
       </c>
       <c r="E126" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D126) / VLOOKUP(C126, tiers, 2, FALSE), "")</f>
-        <v>0.6160714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C126, tiers, 2, FALSE)), "", IF(ISBLANK(D126), -1, 1 - (TODAY() - D126) / VLOOKUP(C126, tiers, 2, FALSE)))</f>
+        <v>0.9017857142857143</v>
       </c>
       <c r="F126" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" s="5"/>
@@ -4454,18 +4047,18 @@
         <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127" s="1">
-        <f ca="1">TODAY() - 44</f>
-        <v>44056</v>
+        <f ca="1">TODAY() - 9</f>
+        <v>44164</v>
       </c>
       <c r="E127" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D127) / VLOOKUP(C127, tiers, 2, FALSE), "")</f>
-        <v>0.60714285714285721</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C127, tiers, 2, FALSE)), "", IF(ISBLANK(D127), -1, 1 - (TODAY() - D127) / VLOOKUP(C127, tiers, 2, FALSE)))</f>
+        <v>0.9196428571428571</v>
       </c>
       <c r="F127" t="s">
         <v>39</v>
@@ -4478,21 +4071,21 @@
         <v>43</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128" s="1">
-        <f ca="1">TODAY() - 45</f>
-        <v>44055</v>
+        <f ca="1">TODAY() - 9</f>
+        <v>44164</v>
       </c>
       <c r="E128" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D128) / VLOOKUP(C128, tiers, 2, FALSE), "")</f>
-        <v>0.5982142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C128, tiers, 2, FALSE)), "", IF(ISBLANK(D128), -1, 1 - (TODAY() - D128) / VLOOKUP(C128, tiers, 2, FALSE)))</f>
+        <v>0.9196428571428571</v>
       </c>
       <c r="F128" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="5"/>
@@ -4502,21 +4095,21 @@
         <v>43</v>
       </c>
       <c r="B129" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" s="1">
-        <f ca="1">TODAY() - 45</f>
-        <v>44055</v>
+        <f ca="1">TODAY() - 9</f>
+        <v>44164</v>
       </c>
       <c r="E129" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D129) / VLOOKUP(C129, tiers, 2, FALSE), "")</f>
-        <v>0.5982142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C129, tiers, 2, FALSE)), "", IF(ISBLANK(D129), -1, 1 - (TODAY() - D129) / VLOOKUP(C129, tiers, 2, FALSE)))</f>
+        <v>0.9196428571428571</v>
       </c>
       <c r="F129" t="s">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="5"/>
@@ -4526,21 +4119,21 @@
         <v>43</v>
       </c>
       <c r="B130" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" s="1">
-        <f ca="1">TODAY() - 46</f>
-        <v>44054</v>
+        <f ca="1">TODAY() - 9</f>
+        <v>44164</v>
       </c>
       <c r="E130" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D130) / VLOOKUP(C130, tiers, 2, FALSE), "")</f>
-        <v>0.5892857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C130, tiers, 2, FALSE)), "", IF(ISBLANK(D130), -1, 1 - (TODAY() - D130) / VLOOKUP(C130, tiers, 2, FALSE)))</f>
+        <v>0.9196428571428571</v>
       </c>
       <c r="F130" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="5"/>
@@ -4550,21 +4143,21 @@
         <v>43</v>
       </c>
       <c r="B131" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131" s="1">
-        <f ca="1">TODAY() - 46</f>
-        <v>44054</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E131" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D131) / VLOOKUP(C131, tiers, 2, FALSE), "")</f>
-        <v>0.5892857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C131, tiers, 2, FALSE)), "", IF(ISBLANK(D131), -1, 1 - (TODAY() - D131) / VLOOKUP(C131, tiers, 2, FALSE)))</f>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F131" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="5"/>
@@ -4574,21 +4167,21 @@
         <v>43</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" s="1">
-        <f ca="1">TODAY() - 47</f>
-        <v>44053</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E132" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D132) / VLOOKUP(C132, tiers, 2, FALSE), "")</f>
-        <v>0.58035714285714279</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C132, tiers, 2, FALSE)), "", IF(ISBLANK(D132), -1, 1 - (TODAY() - D132) / VLOOKUP(C132, tiers, 2, FALSE)))</f>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F132" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="5"/>
@@ -4598,21 +4191,21 @@
         <v>43</v>
       </c>
       <c r="B133" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133" s="1">
-        <f ca="1">TODAY() - 48</f>
-        <v>44052</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E133" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D133) / VLOOKUP(C133, tiers, 2, FALSE), "")</f>
-        <v>0.5714285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C133, tiers, 2, FALSE)), "", IF(ISBLANK(D133), -1, 1 - (TODAY() - D133) / VLOOKUP(C133, tiers, 2, FALSE)))</f>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F133" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G133" s="1"/>
       <c r="H133" s="5"/>
@@ -4622,21 +4215,21 @@
         <v>43</v>
       </c>
       <c r="B134" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134" s="1">
-        <f ca="1">TODAY() - 53</f>
-        <v>44047</v>
+        <f ca="1">TODAY() - 8</f>
+        <v>44165</v>
       </c>
       <c r="E134" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D134) / VLOOKUP(C134, tiers, 2, FALSE), "")</f>
-        <v>0.5267857142857143</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C134, tiers, 2, FALSE)), "", IF(ISBLANK(D134), -1, 1 - (TODAY() - D134) / VLOOKUP(C134, tiers, 2, FALSE)))</f>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F134" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" s="5"/>
@@ -4646,21 +4239,21 @@
         <v>43</v>
       </c>
       <c r="B135" t="s">
-        <v>119</v>
-      </c>
-      <c r="C135">
+        <v>78</v>
+      </c>
+      <c r="C135" s="2">
         <v>1</v>
       </c>
       <c r="D135" s="1">
-        <f ca="1">TODAY() - 55</f>
-        <v>44045</v>
+        <f ca="1">TODAY() - 7</f>
+        <v>44166</v>
       </c>
       <c r="E135" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D135) / VLOOKUP(C135, tiers, 2, FALSE), "")</f>
-        <v>0.5089285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C135, tiers, 2, FALSE)), "", IF(ISBLANK(D135), -1, 1 - (TODAY() - D135) / VLOOKUP(C135, tiers, 2, FALSE)))</f>
+        <v>0.9375</v>
       </c>
       <c r="F135" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" s="5"/>
@@ -4670,21 +4263,21 @@
         <v>43</v>
       </c>
       <c r="B136" t="s">
-        <v>11</v>
-      </c>
-      <c r="C136">
+        <v>77</v>
+      </c>
+      <c r="C136" s="2">
         <v>1</v>
       </c>
       <c r="D136" s="1">
-        <f ca="1">TODAY() - 59</f>
-        <v>44041</v>
+        <f ca="1">TODAY() - 6</f>
+        <v>44167</v>
       </c>
       <c r="E136" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D136) / VLOOKUP(C136, tiers, 2, FALSE), "")</f>
-        <v>0.4732142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C136, tiers, 2, FALSE)), "", IF(ISBLANK(D136), -1, 1 - (TODAY() - D136) / VLOOKUP(C136, tiers, 2, FALSE)))</f>
+        <v>0.9464285714285714</v>
       </c>
       <c r="F136" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" s="5"/>
@@ -4694,21 +4287,21 @@
         <v>43</v>
       </c>
       <c r="B137" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137" s="1">
-        <f ca="1">TODAY() - 62</f>
-        <v>44038</v>
+        <f ca="1">TODAY() - 5</f>
+        <v>44168</v>
       </c>
       <c r="E137" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D137) / VLOOKUP(C137, tiers, 2, FALSE), "")</f>
-        <v>0.4464285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C137, tiers, 2, FALSE)), "", IF(ISBLANK(D137), -1, 1 - (TODAY() - D137) / VLOOKUP(C137, tiers, 2, FALSE)))</f>
+        <v>0.9553571428571429</v>
       </c>
       <c r="F137" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="5"/>
@@ -4718,21 +4311,21 @@
         <v>43</v>
       </c>
       <c r="B138" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138" s="1">
-        <f ca="1">TODAY() - 66</f>
-        <v>44034</v>
+        <f ca="1">TODAY() - 5</f>
+        <v>44168</v>
       </c>
       <c r="E138" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D138) / VLOOKUP(C138, tiers, 2, FALSE), "")</f>
-        <v>0.4107142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C138, tiers, 2, FALSE)), "", IF(ISBLANK(D138), -1, 1 - (TODAY() - D138) / VLOOKUP(C138, tiers, 2, FALSE)))</f>
+        <v>0.9553571428571429</v>
       </c>
       <c r="F138" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" s="5"/>
@@ -4742,21 +4335,21 @@
         <v>43</v>
       </c>
       <c r="B139" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" s="1">
-        <f ca="1">TODAY() - 68</f>
-        <v>44032</v>
+        <f ca="1">TODAY() - 5</f>
+        <v>44168</v>
       </c>
       <c r="E139" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D139) / VLOOKUP(C139, tiers, 2, FALSE), "")</f>
-        <v>0.3928571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C139, tiers, 2, FALSE)), "", IF(ISBLANK(D139), -1, 1 - (TODAY() - D139) / VLOOKUP(C139, tiers, 2, FALSE)))</f>
+        <v>0.9553571428571429</v>
       </c>
       <c r="F139" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" s="5"/>
@@ -4766,21 +4359,21 @@
         <v>43</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140" s="1">
-        <f ca="1">TODAY() - 69</f>
-        <v>44031</v>
+        <f ca="1">TODAY() - 4</f>
+        <v>44169</v>
       </c>
       <c r="E140" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D140) / VLOOKUP(C140, tiers, 2, FALSE), "")</f>
-        <v>0.3839285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C140, tiers, 2, FALSE)), "", IF(ISBLANK(D140), -1, 1 - (TODAY() - D140) / VLOOKUP(C140, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F140" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G140" s="1"/>
       <c r="H140" s="5"/>
@@ -4790,21 +4383,21 @@
         <v>43</v>
       </c>
       <c r="B141" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141" s="1">
-        <f ca="1">TODAY() - 75</f>
-        <v>44025</v>
+        <f ca="1">TODAY() - 4</f>
+        <v>44169</v>
       </c>
       <c r="E141" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D141) / VLOOKUP(C141, tiers, 2, FALSE), "")</f>
-        <v>0.3303571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C141, tiers, 2, FALSE)), "", IF(ISBLANK(D141), -1, 1 - (TODAY() - D141) / VLOOKUP(C141, tiers, 2, FALSE)))</f>
+        <v>0.9642857142857143</v>
       </c>
       <c r="F141" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="5"/>
@@ -4814,21 +4407,21 @@
         <v>43</v>
       </c>
       <c r="B142" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="C142" s="2">
         <v>1</v>
       </c>
       <c r="D142" s="1">
-        <f ca="1">TODAY() - 78</f>
-        <v>44022</v>
+        <f ca="1">TODAY() - 3</f>
+        <v>44170</v>
       </c>
       <c r="E142" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D142) / VLOOKUP(C142, tiers, 2, FALSE), "")</f>
-        <v>0.3035714285714286</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C142, tiers, 2, FALSE)), "", IF(ISBLANK(D142), -1, 1 - (TODAY() - D142) / VLOOKUP(C142, tiers, 2, FALSE)))</f>
+        <v>0.9732142857142857</v>
       </c>
       <c r="F142" t="s">
-        <v>38</v>
+        <v>150</v>
       </c>
       <c r="G142" s="1"/>
       <c r="H142" s="5"/>
@@ -4838,21 +4431,21 @@
         <v>43</v>
       </c>
       <c r="B143" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143" s="1">
-        <f ca="1">TODAY() - 79</f>
-        <v>44021</v>
+        <f ca="1">TODAY() - 3</f>
+        <v>44170</v>
       </c>
       <c r="E143" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D143) / VLOOKUP(C143, tiers, 2, FALSE), "")</f>
-        <v>0.2946428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C143, tiers, 2, FALSE)), "", IF(ISBLANK(D143), -1, 1 - (TODAY() - D143) / VLOOKUP(C143, tiers, 2, FALSE)))</f>
+        <v>0.9732142857142857</v>
       </c>
       <c r="F143" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" s="5"/>
@@ -4862,21 +4455,21 @@
         <v>43</v>
       </c>
       <c r="B144" t="s">
-        <v>145</v>
+        <v>7</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144" s="1">
-        <f ca="1">TODAY() - 82</f>
-        <v>44018</v>
+        <f ca="1">TODAY() - 3</f>
+        <v>44170</v>
       </c>
       <c r="E144" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D144) / VLOOKUP(C144, tiers, 2, FALSE), "")</f>
-        <v>0.2678571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C144, tiers, 2, FALSE)), "", IF(ISBLANK(D144), -1, 1 - (TODAY() - D144) / VLOOKUP(C144, tiers, 2, FALSE)))</f>
+        <v>0.9732142857142857</v>
       </c>
       <c r="F144" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="5"/>
@@ -4886,21 +4479,21 @@
         <v>43</v>
       </c>
       <c r="B145" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145" s="1">
-        <f ca="1">TODAY() - 82</f>
-        <v>44018</v>
+        <f ca="1">TODAY() - 3</f>
+        <v>44170</v>
       </c>
       <c r="E145" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D145) / VLOOKUP(C145, tiers, 2, FALSE), "")</f>
-        <v>0.2678571428571429</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C145, tiers, 2, FALSE)), "", IF(ISBLANK(D145), -1, 1 - (TODAY() - D145) / VLOOKUP(C145, tiers, 2, FALSE)))</f>
+        <v>0.9732142857142857</v>
       </c>
       <c r="F145" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="G145" s="1"/>
       <c r="H145" s="5"/>
@@ -4910,18 +4503,18 @@
         <v>43</v>
       </c>
       <c r="B146" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" s="1">
-        <f ca="1">TODAY() - 86</f>
-        <v>44014</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E146" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D146) / VLOOKUP(C146, tiers, 2, FALSE), "")</f>
-        <v>0.2321428571428571</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C146, tiers, 2, FALSE)), "", IF(ISBLANK(D146), -1, 1 - (TODAY() - D146) / VLOOKUP(C146, tiers, 2, FALSE)))</f>
+        <v>0.9910714285714286</v>
       </c>
       <c r="F146" t="s">
         <v>37</v>
@@ -4934,18 +4527,18 @@
         <v>43</v>
       </c>
       <c r="B147" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" s="1">
-        <f ca="1">TODAY() - 90</f>
-        <v>44010</v>
+        <f ca="1">TODAY() - 1</f>
+        <v>44172</v>
       </c>
       <c r="E147" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D147) / VLOOKUP(C147, tiers, 2, FALSE), "")</f>
-        <v>0.1964285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C147, tiers, 2, FALSE)), "", IF(ISBLANK(D147), -1, 1 - (TODAY() - D147) / VLOOKUP(C147, tiers, 2, FALSE)))</f>
+        <v>0.9910714285714286</v>
       </c>
       <c r="F147" t="s">
         <v>39</v>
@@ -4958,21 +4551,21 @@
         <v>43</v>
       </c>
       <c r="B148" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
       <c r="D148" s="1">
-        <f ca="1">TODAY() - 94</f>
-        <v>44006</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E148" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D148) / VLOOKUP(C148, tiers, 2, FALSE), "")</f>
-        <v>0.1607142857142857</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C148, tiers, 2, FALSE)), "", IF(ISBLANK(D148), -1, 1 - (TODAY() - D148) / VLOOKUP(C148, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="5"/>
@@ -4982,21 +4575,21 @@
         <v>43</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
-      </c>
-      <c r="C149" s="2">
+        <v>15</v>
+      </c>
+      <c r="C149">
         <v>1</v>
       </c>
       <c r="D149" s="1">
-        <f ca="1">TODAY() - 97</f>
-        <v>44003</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E149" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D149) / VLOOKUP(C149, tiers, 2, FALSE), "")</f>
-        <v>0.1339285714285714</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C149, tiers, 2, FALSE)), "", IF(ISBLANK(D149), -1, 1 - (TODAY() - D149) / VLOOKUP(C149, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F149" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G149" s="1"/>
       <c r="H149" s="5"/>
@@ -5006,21 +4599,21 @@
         <v>43</v>
       </c>
       <c r="B150" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150" s="1">
-        <f ca="1">TODAY() - 102</f>
-        <v>43998</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E150" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D150) / VLOOKUP(C150, tiers, 2, FALSE), "")</f>
-        <v>8.9285714285714302E-2</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C150, tiers, 2, FALSE)), "", IF(ISBLANK(D150), -1, 1 - (TODAY() - D150) / VLOOKUP(C150, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="5"/>
@@ -5030,40 +4623,40 @@
         <v>43</v>
       </c>
       <c r="B151" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" s="1">
-        <f ca="1">TODAY() - 108</f>
-        <v>43992</v>
+        <f ca="1">TODAY() - 0</f>
+        <v>44173</v>
       </c>
       <c r="E151" s="3">
-        <f ca="1">_xlfn.IFNA(1 - (TODAY() - D151) / VLOOKUP(C151, tiers, 2, FALSE), "")</f>
-        <v>3.5714285714285698E-2</v>
+        <f ca="1">IF(ISNA(VLOOKUP(C151, tiers, 2, FALSE)), "", IF(ISBLANK(D151), -1, 1 - (TODAY() - D151) / VLOOKUP(C151, tiers, 2, FALSE)))</f>
+        <v>1</v>
       </c>
       <c r="F151" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="G151" s="1"/>
       <c r="H151" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H151">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
     <sortCondition descending="1" ref="C2:C151"/>
-    <sortCondition descending="1" ref="D2:D151"/>
+    <sortCondition ref="D2:D151"/>
     <sortCondition ref="B2:B151"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="between">
       <formula>0</formula>
       <formula>0.2</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="11">
+    <cfRule type="containsBlanks" dxfId="6" priority="11">
       <formula>LEN(TRIM(E1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5076,7 +4669,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5093,20 +4686,20 @@
     <row r="2" spans="1:1" ht="25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <f ca="1">AVERAGE(recency)</f>
-        <v>0.71124999999999994</v>
+        <v>0.71125000000000005</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="lessThan">
-      <formula>0.45</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="between">
-      <formula>0.45</formula>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>0.5</formula>
+      <formula>0.55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>0.55</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>